<commit_message>
sigh couldn't go back to corins-edit branch
</commit_message>
<xml_diff>
--- a/Testing/data/where-to-focus-v3.xlsx
+++ b/Testing/data/where-to-focus-v3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliver.g.alexander\Projects\remote-workshop\Testing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1337346-33C3-4E77-A9AB-6B6537A62C86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3822C875-148E-4427-8AA9-D1B3D00A1A0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="where-to-focus-v2" sheetId="1" r:id="rId1"/>
@@ -97,20 +97,20 @@
     <t>Transparency and accuracy in the reporting of financial health and other business metrics.</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Self nominated category</t>
-  </si>
-  <si>
     <t>Environmental</t>
+  </si>
+  <si>
+    <t>A workplace which fosters and supports diversity, inclusiveness</t>
+  </si>
+  <si>
+    <t>Support and develop employees to help individuals reach their full potential and improve outcomes for the company</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +241,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -587,8 +594,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -943,14 +951,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -965,7 +977,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -976,7 +988,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -992,6 +1004,9 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1011,6 +1026,9 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1078,15 +1096,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>